<commit_message>
débuts de rapport dans le readme
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\320\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\320\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B2A92D-84C0-4195-9316-F071DCE1767F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30FC3AE-D2C2-43CA-B918-188D4D24C434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Auteur:</t>
   </si>
@@ -112,6 +112,9 @@
   <si>
     <t>Création de l'illustration du jeu</t>
   </si>
+  <si>
+    <t>Création de l'illustration du jeu sur figma</t>
+  </si>
 </sst>
 </file>
 
@@ -119,9 +122,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-CH,1]dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="0\ &quot;h&quot;"/>
-    <numFmt numFmtId="167" formatCode="dd\ mmm"/>
-    <numFmt numFmtId="168" formatCode="00\ &quot;min&quot;"/>
+    <numFmt numFmtId="165" formatCode="0\ &quot;h&quot;"/>
+    <numFmt numFmtId="166" formatCode="dd\ mmm"/>
+    <numFmt numFmtId="167" formatCode="00\ &quot;min&quot;"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -299,39 +302,39 @@
     <xf numFmtId="20" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -366,7 +369,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -541,7 +544,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="00\ &quot;min&quot;"/>
+      <numFmt numFmtId="167" formatCode="00\ &quot;min&quot;"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -562,7 +565,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="0\ &quot;h&quot;"/>
+      <numFmt numFmtId="165" formatCode="0\ &quot;h&quot;"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -582,7 +585,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="dd\ mmm"/>
+      <numFmt numFmtId="166" formatCode="dd\ mmm"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -877,9 +880,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -934,7 +937,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>2 heures 30 minutes</v>
+        <v>3 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -953,11 +956,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1014,11 +1017,13 @@
       <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="str">
+      <c r="A8" s="39">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="27"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="27">
+        <v>45678</v>
+      </c>
       <c r="C8" s="28"/>
       <c r="D8" s="29">
         <v>30</v>
@@ -1041,11 +1046,13 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="str">
+      <c r="A9" s="40">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="31"/>
+        <v>4</v>
+      </c>
+      <c r="B9" s="31">
+        <v>45678</v>
+      </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33">
         <v>30</v>
@@ -1068,15 +1075,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="str">
+      <c r="A10" s="39">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="27"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="27">
+        <v>45678</v>
+      </c>
       <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="20"/>
+      <c r="D10" s="29">
+        <v>30</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>24</v>
+      </c>
       <c r="G10" s="36"/>
       <c r="M10" t="s">
         <v>3</v>
@@ -7437,7 +7452,7 @@
       <formula>$E7="Implémentation"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C532" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
       <formula1>$N$7:$N$15</formula1>
     </dataValidation>
@@ -7658,6 +7673,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -7666,15 +7690,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7697,6 +7712,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7707,12 +7730,4 @@
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(readme): ajout de l'intro et planification
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\320\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30FC3AE-D2C2-43CA-B918-188D4D24C434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F403CAA1-0180-40A4-AF30-8310EAB5E8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Journal de travail'!$A$6:$G$6</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Auteur:</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Création de l'illustration du jeu sur figma</t>
+  </si>
+  <si>
+    <t>Céation des user stories.</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport</t>
   </si>
 </sst>
 </file>
@@ -882,7 +888,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -937,7 +943,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>3 heures 0 minutes</v>
+        <v>6 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -952,15 +958,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -997,10 +1003,10 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B7" s="23">
-        <v>45678</v>
+        <v>45927</v>
       </c>
       <c r="C7" s="24">
         <v>1</v>
@@ -1019,10 +1025,10 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B8" s="27">
-        <v>45678</v>
+        <v>45927</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="29">
@@ -1048,10 +1054,10 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B9" s="31">
-        <v>45678</v>
+        <v>45927</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33">
@@ -1077,10 +1083,10 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B10" s="27">
-        <v>45678</v>
+        <v>45927</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="29">
@@ -1104,15 +1110,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="str">
+      <c r="A11" s="40">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="31"/>
+        <v>36</v>
+      </c>
+      <c r="B11" s="31">
+        <v>45903</v>
+      </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="33">
+        <v>30</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="37"/>
       <c r="M11" t="s">
         <v>4</v>
@@ -1125,15 +1139,25 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="str">
+      <c r="A12" s="39">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="20"/>
+        <v>36</v>
+      </c>
+      <c r="B12" s="27">
+        <v>45903</v>
+      </c>
+      <c r="C12" s="28">
+        <v>1</v>
+      </c>
+      <c r="D12" s="29">
+        <v>30</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="G12" s="36"/>
       <c r="M12" t="s">
         <v>17</v>
@@ -1146,15 +1170,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="str">
+      <c r="A13" s="40">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
+        <v>36</v>
+      </c>
+      <c r="B13" s="31">
+        <v>45903</v>
+      </c>
+      <c r="C13" s="32">
+        <v>1</v>
+      </c>
       <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="G13" s="37"/>
       <c r="N13">
         <v>6</v>
@@ -7452,7 +7484,7 @@
       <formula>$E7="Implémentation"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C532" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
       <formula1>$N$7:$N$15</formula1>
     </dataValidation>
@@ -7673,15 +7705,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -7690,6 +7713,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7712,14 +7744,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7730,4 +7754,12 @@
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore(jdt): précision des tâches
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\320\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F403CAA1-0180-40A4-AF30-8310EAB5E8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6FB512-BE1A-4695-8C4C-736FF2CA90BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3405" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Auteur:</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Rédaction du rapport</t>
+  </si>
+  <si>
+    <t>Documentation en lien avec markdown.</t>
+  </si>
+  <si>
+    <t>Expliquations à propos du cdc, git, etc</t>
+  </si>
+  <si>
+    <t>Expliquations sur l'utilisation de figma.</t>
   </si>
 </sst>
 </file>
@@ -886,9 +895,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -943,7 +952,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 0 minutes</v>
+        <v>6 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -958,15 +967,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>360</v>
+        <v>390</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1020,7 +1029,9 @@
       <c r="F7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="35" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
@@ -1127,7 +1138,9 @@
       <c r="F11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="37" t="s">
+        <v>29</v>
+      </c>
       <c r="M11" t="s">
         <v>4</v>
       </c>
@@ -1177,15 +1190,15 @@
       <c r="B13" s="31">
         <v>45903</v>
       </c>
-      <c r="C13" s="32">
-        <v>1</v>
-      </c>
-      <c r="D13" s="33"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33">
+        <v>40</v>
+      </c>
       <c r="E13" s="34" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G13" s="37"/>
       <c r="N13">
@@ -1196,15 +1209,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="str">
+      <c r="A14" s="39">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="27"/>
+        <v>36</v>
+      </c>
+      <c r="B14" s="27">
+        <v>45903</v>
+      </c>
       <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="29">
+        <v>50</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="G14" s="36"/>
       <c r="N14">
         <v>7</v>
@@ -7705,6 +7726,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -7713,15 +7743,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7744,6 +7765,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7754,12 +7783,4 @@
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(player): permière implementation des mouvements
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\320\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Module\320\shootthemup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6FB512-BE1A-4695-8C4C-736FF2CA90BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7DC3C8-EE4E-4F1A-9F79-9E409DC62D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3405" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Auteur:</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Expliquations sur l'utilisation de figma.</t>
+  </si>
+  <si>
+    <t>Modifcation des userstories pour qu'elles soient conforme avec les remarques du prof.</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je refais l'exos drones pour bien comprendre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je ne savais pas quoi faire je ne comprennais rien au forms </t>
   </si>
 </sst>
 </file>
@@ -897,7 +909,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -952,7 +964,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 30 minutes</v>
+        <v>11 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -967,15 +979,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>360</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>390</v>
+        <v>660</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1235,15 +1247,25 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="str">
+      <c r="A15" s="40">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="20"/>
+        <v>37</v>
+      </c>
+      <c r="B15" s="31">
+        <v>45910</v>
+      </c>
+      <c r="C15" s="32">
+        <v>1</v>
+      </c>
+      <c r="D15" s="33">
+        <v>30</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G15" s="37"/>
       <c r="N15">
         <v>8</v>
@@ -1253,30 +1275,44 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="str">
+      <c r="A16" s="39">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
+        <v>38</v>
+      </c>
+      <c r="B16" s="27">
+        <v>45917</v>
+      </c>
+      <c r="C16" s="28">
+        <v>2</v>
+      </c>
       <c r="D16" s="29"/>
       <c r="E16" s="30"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="36"/>
+      <c r="F16" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="str">
+      <c r="A17" s="40">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
+        <v>38</v>
+      </c>
+      <c r="B17" s="31">
+        <v>45917</v>
+      </c>
+      <c r="C17" s="32">
+        <v>1</v>
+      </c>
       <c r="D17" s="33"/>
       <c r="E17" s="34"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="G17" s="37"/>
       <c r="O17">
         <v>45</v>
@@ -7525,6 +7561,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -7725,15 +7770,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7746,6 +7782,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7764,14 +7808,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat(player): modification des mouvements pour plus de fluidité
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Module\320\shootthemup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7DC3C8-EE4E-4F1A-9F79-9E409DC62D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEC7DFE-78E3-479B-8D08-ECC8947545A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3405" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Auteur:</t>
   </si>
@@ -134,13 +134,22 @@
     <t>Modifcation des userstories pour qu'elles soient conforme avec les remarques du prof.</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t xml:space="preserve">Je refais l'exos drones pour bien comprendre </t>
   </si>
   <si>
     <t xml:space="preserve">Je ne savais pas quoi faire je ne comprennais rien au forms </t>
+  </si>
+  <si>
+    <t>Documentation en lien avec les forms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reprise de l'exo drones dans le projet </t>
+  </si>
+  <si>
+    <t>Ajout des mouvements</t>
+  </si>
+  <si>
+    <t>Prise de connaissance des conventions de codage</t>
   </si>
 </sst>
 </file>
@@ -908,8 +917,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -964,7 +973,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>11 heures 0 minutes</v>
+        <v>13 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -979,15 +988,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>660</v>
+        <v>780</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1286,12 +1295,14 @@
         <v>2</v>
       </c>
       <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
+      <c r="E16" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="F16" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O16">
         <v>40</v>
@@ -1309,9 +1320,11 @@
         <v>1</v>
       </c>
       <c r="D17" s="33"/>
-      <c r="E17" s="34"/>
+      <c r="E17" s="34" t="s">
+        <v>2</v>
+      </c>
       <c r="F17" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17" s="37"/>
       <c r="O17">
@@ -1319,45 +1332,69 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="str">
+      <c r="A18" s="39">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
+        <v>39</v>
+      </c>
+      <c r="B18" s="27">
+        <v>45924</v>
+      </c>
+      <c r="C18" s="28">
+        <v>1</v>
+      </c>
       <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="20"/>
+      <c r="E18" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="G18" s="36"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="str">
+      <c r="A19" s="40">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="31"/>
+        <v>39</v>
+      </c>
+      <c r="B19" s="31">
+        <v>45924</v>
+      </c>
       <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="20"/>
+      <c r="D19" s="33">
+        <v>30</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="G19" s="37"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="str">
+      <c r="A20" s="39">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="27"/>
+        <v>39</v>
+      </c>
+      <c r="B20" s="27">
+        <v>45923</v>
+      </c>
       <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="20"/>
+      <c r="D20" s="29">
+        <v>30</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="G20" s="36"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -7561,15 +7598,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -7770,6 +7798,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7782,14 +7819,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7808,6 +7837,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat(mouvement): suppression du 2e timer et set de la position y du joueur relativement a la taille de la fenetre
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Module\320\shootthemup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEC7DFE-78E3-479B-8D08-ECC8947545A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D77586D-5C14-47E1-81B6-E51AC770C38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3405" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Auteur:</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Prise de connaissance des conventions de codage</t>
+  </si>
+  <si>
+    <t>Suppression du 2e timer et mise en forme du code en conséquance</t>
+  </si>
+  <si>
+    <t>j'ai enfin compris comment la methode NewFrame est appelée</t>
   </si>
 </sst>
 </file>
@@ -918,7 +924,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -973,7 +979,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>13 heures 0 minutes</v>
+        <v>14 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -988,7 +994,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -996,7 +1002,7 @@
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>780</v>
+        <v>840</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1383,7 +1389,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="27">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="29">
@@ -1398,16 +1404,26 @@
       <c r="G20" s="36"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="str">
+      <c r="A21" s="40">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32"/>
+        <v>39</v>
+      </c>
+      <c r="B21" s="31">
+        <v>45924</v>
+      </c>
+      <c r="C21" s="32">
+        <v>1</v>
+      </c>
       <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="37"/>
+      <c r="E21" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="39" t="str">

</xml_diff>

<commit_message>
feat(enemies): Ajout des classes view et modèle des ennemis
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Module\320\shootthemup\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn26qvj\Desktop\shootthemup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D77586D-5C14-47E1-81B6-E51AC770C38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335B12CF-ADEA-4887-9032-C0786E9FE6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="1665" yWindow="1350" windowWidth="23685" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Auteur:</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>j'ai enfin compris comment la methode NewFrame est appelée</t>
+  </si>
+  <si>
+    <t>Comment dessiner des fonctions sur un form</t>
   </si>
 </sst>
 </file>
@@ -979,7 +982,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>14 heures 0 minutes</v>
+        <v>15 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -994,15 +997,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>480</v>
+        <v>540</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>360</v>
+        <v>390</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>840</v>
+        <v>930</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1426,15 +1429,25 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="str">
+      <c r="A22" s="39">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="B22" s="27">
+        <v>45931</v>
+      </c>
+      <c r="C22" s="28">
+        <v>1</v>
+      </c>
+      <c r="D22" s="29">
+        <v>30</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -7614,6 +7627,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -7814,15 +7836,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7835,6 +7848,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7853,14 +7874,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat(ennemis): ajout d'un mouvement des ennemis WOP
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn26qvj\Desktop\shootthemup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335B12CF-ADEA-4887-9032-C0786E9FE6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7946C884-E321-4391-B414-74839B6FCE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="1350" windowWidth="23685" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Auteur:</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Comment dessiner des fonctions sur un form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Débuts dans la création des ennemis </t>
   </si>
 </sst>
 </file>
@@ -927,7 +930,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -982,7 +985,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>15 heures 30 minutes</v>
+        <v>17 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -997,15 +1000,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>540</v>
+        <v>600</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>390</v>
+        <v>420</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>930</v>
+        <v>1020</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1451,15 +1454,25 @@
       <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="str">
+      <c r="A23" s="40">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="B23" s="31">
+        <v>45931</v>
+      </c>
+      <c r="C23" s="32">
+        <v>1</v>
+      </c>
+      <c r="D23" s="33">
+        <v>30</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -7627,15 +7640,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -7836,6 +7840,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7848,14 +7861,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7874,6 +7879,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
doc(jdt): modification du jdt
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn26qvj\Desktop\shootthemup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7946C884-E321-4391-B414-74839B6FCE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0128668-5F02-431F-BA7C-0C0F8BA8F332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="1350" windowWidth="23685" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="870" yWindow="330" windowWidth="24480" windowHeight="14925" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Auteur:</t>
   </si>
@@ -162,6 +162,21 @@
   </si>
   <si>
     <t xml:space="preserve">Débuts dans la création des ennemis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification du nom de projet </t>
+  </si>
+  <si>
+    <t>Réponse au mail de M.Sahli</t>
+  </si>
+  <si>
+    <t>Modifcations mineures sur joueur et modification des textures</t>
+  </si>
+  <si>
+    <t>Finalisation de la US sur les ennemis</t>
+  </si>
+  <si>
+    <t>Ajout des projectiles</t>
   </si>
 </sst>
 </file>
@@ -928,9 +943,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -985,7 +1000,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>17 heures 0 minutes</v>
+        <v>20 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -1004,11 +1019,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>1020</v>
+        <v>1200</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1045,10 +1060,10 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" s="23">
-        <v>45927</v>
+        <v>45896</v>
       </c>
       <c r="C7" s="24">
         <v>1</v>
@@ -1069,10 +1084,10 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" s="27">
-        <v>45927</v>
+        <v>45896</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="29">
@@ -1098,10 +1113,10 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" s="31">
-        <v>45927</v>
+        <v>45896</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33">
@@ -1127,10 +1142,10 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" s="27">
-        <v>45927</v>
+        <v>45896</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="29">
@@ -1154,26 +1169,16 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
+      <c r="A11" s="40" t="str">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v>36</v>
-      </c>
-      <c r="B11" s="31">
-        <v>45903</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B11" s="31"/>
       <c r="C11" s="32"/>
-      <c r="D11" s="33">
-        <v>30</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>29</v>
-      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="37"/>
       <c r="M11" t="s">
         <v>4</v>
       </c>
@@ -1192,19 +1197,19 @@
       <c r="B12" s="27">
         <v>45903</v>
       </c>
-      <c r="C12" s="28">
-        <v>1</v>
-      </c>
+      <c r="C12" s="28"/>
       <c r="D12" s="29">
         <v>30</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="36"/>
+        <v>21</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>29</v>
+      </c>
       <c r="M12" t="s">
         <v>17</v>
       </c>
@@ -1223,15 +1228,17 @@
       <c r="B13" s="31">
         <v>45903</v>
       </c>
-      <c r="C13" s="32"/>
+      <c r="C13" s="32">
+        <v>1</v>
+      </c>
       <c r="D13" s="33">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G13" s="37"/>
       <c r="N13">
@@ -1251,13 +1258,13 @@
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="29">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G14" s="36"/>
       <c r="N14">
@@ -1270,22 +1277,20 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="31">
-        <v>45910</v>
-      </c>
-      <c r="C15" s="32">
-        <v>1</v>
-      </c>
+        <v>45903</v>
+      </c>
+      <c r="C15" s="32"/>
       <c r="D15" s="33">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G15" s="37"/>
       <c r="N15">
@@ -1296,26 +1301,16 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="39">
+      <c r="A16" s="39" t="str">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v>38</v>
-      </c>
-      <c r="B16" s="27">
-        <v>45917</v>
-      </c>
-      <c r="C16" s="28">
-        <v>2</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="29"/>
-      <c r="E16" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>32</v>
-      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="36"/>
       <c r="O16">
         <v>40</v>
       </c>
@@ -1323,20 +1318,22 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="31">
-        <v>45917</v>
+        <v>45910</v>
       </c>
       <c r="C17" s="32">
         <v>1</v>
       </c>
-      <c r="D17" s="33"/>
+      <c r="D17" s="33">
+        <v>30</v>
+      </c>
       <c r="E17" s="34" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="37"/>
       <c r="O17">
@@ -1344,23 +1341,15 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
+      <c r="A18" s="39" t="str">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v>39</v>
-      </c>
-      <c r="B18" s="27">
-        <v>45924</v>
-      </c>
-      <c r="C18" s="28">
-        <v>1</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="29"/>
-      <c r="E18" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>34</v>
-      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="36"/>
       <c r="O18">
         <v>50</v>
@@ -1369,22 +1358,24 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="31">
-        <v>45924</v>
-      </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33">
-        <v>30</v>
-      </c>
+        <v>45917</v>
+      </c>
+      <c r="C19" s="32">
+        <v>2</v>
+      </c>
+      <c r="D19" s="33"/>
       <c r="E19" s="34" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="37"/>
+        <v>33</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>32</v>
+      </c>
       <c r="O19">
         <v>55</v>
       </c>
@@ -1392,78 +1383,64 @@
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="27">
-        <v>45924</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29">
-        <v>30</v>
-      </c>
+        <v>45917</v>
+      </c>
+      <c r="C20" s="28">
+        <v>1</v>
+      </c>
+      <c r="D20" s="29"/>
       <c r="E20" s="30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G20" s="36"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="40">
+      <c r="A21" s="40" t="str">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v>39</v>
-      </c>
-      <c r="B21" s="31">
-        <v>45924</v>
-      </c>
-      <c r="C21" s="32">
-        <v>1</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="33"/>
-      <c r="E21" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>38</v>
-      </c>
+      <c r="E21" s="34"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="37"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="27">
-        <v>45931</v>
+        <v>45924</v>
       </c>
       <c r="C22" s="28">
         <v>1</v>
       </c>
-      <c r="D22" s="29">
-        <v>30</v>
-      </c>
+      <c r="D22" s="29"/>
       <c r="E22" s="30" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="31">
-        <v>45931</v>
-      </c>
-      <c r="C23" s="32">
-        <v>1</v>
-      </c>
+        <v>45924</v>
+      </c>
+      <c r="C23" s="32"/>
       <c r="D23" s="33">
         <v>30</v>
       </c>
@@ -1471,33 +1448,51 @@
         <v>14</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="str">
+      <c r="A24" s="39">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="27"/>
+        <v>39</v>
+      </c>
+      <c r="B24" s="27">
+        <v>45924</v>
+      </c>
       <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="20"/>
+      <c r="D24" s="29">
+        <v>30</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="G24" s="36"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="str">
+      <c r="A25" s="40">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="32"/>
+        <v>39</v>
+      </c>
+      <c r="B25" s="31">
+        <v>45924</v>
+      </c>
+      <c r="C25" s="32">
+        <v>1</v>
+      </c>
       <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="37"/>
+      <c r="E25" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="39" t="str">
@@ -1512,27 +1507,47 @@
       <c r="G26" s="36"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="str">
+      <c r="A27" s="40">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="B27" s="31">
+        <v>45931</v>
+      </c>
+      <c r="C27" s="32">
+        <v>1</v>
+      </c>
+      <c r="D27" s="33">
+        <v>30</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="G27" s="37"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="str">
+      <c r="A28" s="39">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="B28" s="27">
+        <v>45931</v>
+      </c>
+      <c r="C28" s="28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="29">
+        <v>30</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>40</v>
+      </c>
       <c r="G28" s="36"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1548,75 +1563,123 @@
       <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="str">
+      <c r="A30" s="39">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="B30" s="27">
+        <v>45938</v>
+      </c>
       <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="20"/>
+      <c r="D30" s="29">
+        <v>20</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G30" s="36"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="str">
+      <c r="A31" s="40">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="B31" s="31">
+        <v>45938</v>
+      </c>
       <c r="C31" s="32"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="19"/>
+      <c r="D31" s="33">
+        <v>20</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="str">
+      <c r="A32" s="39">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="B32" s="27">
+        <v>45938</v>
+      </c>
       <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="20"/>
+      <c r="D32" s="29">
+        <v>50</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="G32" s="36"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="40" t="str">
+      <c r="A33" s="40">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="B33" s="31">
+        <v>45938</v>
+      </c>
       <c r="C33" s="32"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="19"/>
+      <c r="D33" s="33">
+        <v>15</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="G33" s="37"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="str">
+      <c r="A34" s="39">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="B34" s="27">
+        <v>45938</v>
+      </c>
       <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="19"/>
+      <c r="D34" s="29">
+        <v>30</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="G34" s="36"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="40" t="str">
+      <c r="A35" s="40">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="B35" s="31">
+        <v>45938</v>
+      </c>
       <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="20"/>
+      <c r="D35" s="33">
+        <v>45</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="G35" s="37"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -7640,6 +7703,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -7840,15 +7912,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7861,6 +7924,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7879,14 +7950,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat(player, ennemy): modification du render
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn26qvj\Desktop\shootthemup\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\VS2022\shootthemup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB22A998-C205-4B4D-9BF7-D3E92E04C025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED8F207-779F-4D2F-B65F-FEA668A4DB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="675" windowWidth="24480" windowHeight="14925" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>Auteur:</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>les ennemis tirent le meme nombre de charges que il y a d'ennemis (16h01)</t>
+  </si>
+  <si>
+    <t>Redéplacement des listes au bon endroit et nettoyage de tout le code</t>
+  </si>
+  <si>
+    <t>Les classes view n'existent plus le render et les updates se font dans model</t>
+  </si>
+  <si>
+    <t>Ajout des colisions</t>
+  </si>
+  <si>
+    <t>Ajout des boucliers pour arriver au look final du jeu</t>
   </si>
 </sst>
 </file>
@@ -957,10 +969,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.875" style="1" customWidth="1"/>
@@ -1012,7 +1024,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>23 heures 0 minutes</v>
+        <v>27 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -1027,7 +1039,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>780</v>
+        <v>1020</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -1035,7 +1047,7 @@
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>1380</v>
+        <v>1620</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1715,11 +1727,11 @@
         <v>45959</v>
       </c>
       <c r="C37" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="33"/>
       <c r="E37" s="34" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F37" s="19" t="s">
         <v>46</v>
@@ -1737,7 +1749,7 @@
         <v>45959</v>
       </c>
       <c r="C38" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="30" t="s">
@@ -1763,16 +1775,26 @@
       <c r="G39" s="37"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="str">
+      <c r="A40" s="39">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
+        <v>44</v>
+      </c>
+      <c r="B40" s="27">
+        <v>45961</v>
+      </c>
+      <c r="C40" s="28">
+        <v>2</v>
+      </c>
       <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="36"/>
+      <c r="E40" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" s="36" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="str">
@@ -1787,15 +1809,23 @@
       <c r="G41" s="37"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="str">
+      <c r="A42" s="39">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="28"/>
+        <v>40</v>
+      </c>
+      <c r="B42" s="27">
+        <v>45931</v>
+      </c>
+      <c r="C42" s="28">
+        <v>1</v>
+      </c>
       <c r="D42" s="29"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="19"/>
+      <c r="E42" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="G42" s="36"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1804,10 +1834,16 @@
         <v/>
       </c>
       <c r="B43" s="31"/>
-      <c r="C43" s="32"/>
+      <c r="C43" s="32">
+        <v>1</v>
+      </c>
       <c r="D43" s="33"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="19"/>
+      <c r="E43" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>53</v>
+      </c>
       <c r="G43" s="37"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -7936,15 +7972,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -7953,6 +7980,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7975,14 +8011,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7993,4 +8021,12 @@
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore(projet): rédaction du rapport et préparation à la livraison
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BraimiAlbert.xlsx
+++ b/doc/Journal-de-Travail_BraimiAlbert.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\VS2022\shootthemup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED8F207-779F-4D2F-B65F-FEA668A4DB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71914792-24AA-4A5A-9062-73CA8C655DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="4710" yWindow="2955" windowWidth="28800" windowHeight="17145" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Journal de travail'!$A$6:$G$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$B$7:$G$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>Auteur:</t>
   </si>
@@ -201,6 +202,24 @@
   </si>
   <si>
     <t>Ajout des boucliers pour arriver au look final du jeu</t>
+  </si>
+  <si>
+    <t>Modification des hitbox</t>
+  </si>
+  <si>
+    <t>Ajout des obstacles</t>
+  </si>
+  <si>
+    <t>Ajout des colisions et bloquages avec les obstacles</t>
+  </si>
+  <si>
+    <t>Modification de la manière de générer les ennemis</t>
+  </si>
+  <si>
+    <t>J'ai essayé de faire une forme de génération procédurale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout de tout les commentaires dans le code </t>
   </si>
 </sst>
 </file>
@@ -969,7 +988,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1043,7 @@
       <c r="B3" s="46"/>
       <c r="C3" s="43" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>27 heures 0 minutes</v>
+        <v>35 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -1039,15 +1058,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>1020</v>
+        <v>1440</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>600</v>
+        <v>660</v>
       </c>
       <c r="E4" s="21">
         <f>SUM(C4:D4)</f>
-        <v>1620</v>
+        <v>2100</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -1811,10 +1830,10 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="39">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B42" s="27">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C42" s="28">
         <v>1</v>
@@ -1829,11 +1848,13 @@
       <c r="G42" s="36"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="str">
+      <c r="A43" s="40">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="31"/>
+        <v>44</v>
+      </c>
+      <c r="B43" s="31">
+        <v>45962</v>
+      </c>
       <c r="C43" s="32">
         <v>1</v>
       </c>
@@ -1847,15 +1868,23 @@
       <c r="G43" s="37"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="str">
+      <c r="A44" s="39">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="28"/>
+        <v>44</v>
+      </c>
+      <c r="B44" s="27">
+        <v>45962</v>
+      </c>
+      <c r="C44" s="28">
+        <v>1</v>
+      </c>
       <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="19"/>
+      <c r="E44" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>54</v>
+      </c>
       <c r="G44" s="36"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1871,63 +1900,107 @@
       <c r="G45" s="37"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="str">
+      <c r="A46" s="39">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v/>
-      </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="27">
+        <v>45963</v>
+      </c>
+      <c r="C46" s="28">
+        <v>2</v>
+      </c>
       <c r="D46" s="29"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="19"/>
+      <c r="E46" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="G46" s="36"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="40" t="str">
+      <c r="A47" s="40">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="31"/>
+        <v>44</v>
+      </c>
+      <c r="B47" s="31">
+        <v>45963</v>
+      </c>
       <c r="C47" s="32"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="19"/>
+      <c r="D47" s="33">
+        <v>30</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>56</v>
+      </c>
       <c r="G47" s="37"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="str">
+      <c r="A48" s="39">
         <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
-        <v/>
-      </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="28"/>
+        <v>44</v>
+      </c>
+      <c r="B48" s="27">
+        <v>45963</v>
+      </c>
+      <c r="C48" s="28">
+        <v>2</v>
+      </c>
       <c r="D48" s="29"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="36"/>
+      <c r="E48" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G48" s="36" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="40" t="str">
+      <c r="A49" s="40">
         <f>IF(ISBLANK(B49),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B49))</f>
-        <v/>
-      </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="32"/>
+        <v>44</v>
+      </c>
+      <c r="B49" s="31">
+        <v>45963</v>
+      </c>
+      <c r="C49" s="32">
+        <v>1</v>
+      </c>
       <c r="D49" s="33"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="19"/>
+      <c r="E49" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="G49" s="37"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="str">
+      <c r="A50" s="39">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B50))</f>
-        <v/>
-      </c>
-      <c r="B50" s="27"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="19"/>
+        <v>44</v>
+      </c>
+      <c r="B50" s="27">
+        <v>45963</v>
+      </c>
+      <c r="C50" s="28">
+        <v>1</v>
+      </c>
+      <c r="D50" s="29">
+        <v>30</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="G50" s="36"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -7762,8 +7835,8 @@
       <formula1>$M$7:$M$12</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -8013,12 +8086,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>